<commit_message>
- update date error in bbourecruit_a
</commit_message>
<xml_diff>
--- a/data-raw/recruitment.xlsx
+++ b/data-raw/recruitment.xlsx
@@ -5627,7 +5627,7 @@
         <v>2</v>
       </c>
       <c r="D170">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E170">
         <v>3</v>
@@ -5658,7 +5658,7 @@
         <v>2</v>
       </c>
       <c r="D171">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E171">
         <v>2</v>
@@ -5689,7 +5689,7 @@
         <v>2</v>
       </c>
       <c r="D172">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E172">
         <v>4</v>
@@ -5720,7 +5720,7 @@
         <v>2</v>
       </c>
       <c r="D173">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E173">
         <v>4</v>
@@ -5751,7 +5751,7 @@
         <v>2</v>
       </c>
       <c r="D174">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E174">
         <v>3</v>
@@ -5782,7 +5782,7 @@
         <v>2</v>
       </c>
       <c r="D175">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -5813,7 +5813,7 @@
         <v>2</v>
       </c>
       <c r="D176">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E176">
         <v>5</v>
@@ -5844,7 +5844,7 @@
         <v>2</v>
       </c>
       <c r="D177">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E177">
         <v>3</v>
@@ -5875,7 +5875,7 @@
         <v>2</v>
       </c>
       <c r="D178">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E178">
         <v>2</v>
@@ -5906,7 +5906,7 @@
         <v>2</v>
       </c>
       <c r="D179">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E179">
         <v>5</v>
@@ -5937,7 +5937,7 @@
         <v>2</v>
       </c>
       <c r="D180">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E180">
         <v>5</v>
@@ -5968,7 +5968,7 @@
         <v>2</v>
       </c>
       <c r="D181">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E181">
         <v>5</v>
@@ -5999,7 +5999,7 @@
         <v>2</v>
       </c>
       <c r="D182">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E182">
         <v>4</v>
@@ -6030,7 +6030,7 @@
         <v>2</v>
       </c>
       <c r="D183">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E183">
         <v>3</v>
@@ -6061,7 +6061,7 @@
         <v>2</v>
       </c>
       <c r="D184">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -6092,7 +6092,7 @@
         <v>2</v>
       </c>
       <c r="D185">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E185">
         <v>5</v>
@@ -6123,7 +6123,7 @@
         <v>2</v>
       </c>
       <c r="D186">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E186">
         <v>4</v>
@@ -6154,7 +6154,7 @@
         <v>2</v>
       </c>
       <c r="D187">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E187">
         <v>3</v>
@@ -6185,7 +6185,7 @@
         <v>2</v>
       </c>
       <c r="D188">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E188">
         <v>2</v>
@@ -6216,7 +6216,7 @@
         <v>2</v>
       </c>
       <c r="D189">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E189">
         <v>2</v>
@@ -6247,7 +6247,7 @@
         <v>2</v>
       </c>
       <c r="D190">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E190">
         <v>3</v>
@@ -6278,7 +6278,7 @@
         <v>2</v>
       </c>
       <c r="D191">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E191">
         <v>4</v>
@@ -6309,7 +6309,7 @@
         <v>2</v>
       </c>
       <c r="D192">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E192">
         <v>6</v>
@@ -6340,7 +6340,7 @@
         <v>2</v>
       </c>
       <c r="D193">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E193">
         <v>4</v>
@@ -6371,7 +6371,7 @@
         <v>2</v>
       </c>
       <c r="D194">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E194">
         <v>3</v>
@@ -6402,7 +6402,7 @@
         <v>2</v>
       </c>
       <c r="D195">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E195">
         <v>4</v>
@@ -6433,7 +6433,7 @@
         <v>2</v>
       </c>
       <c r="D196">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E196">
         <v>2</v>
@@ -6464,7 +6464,7 @@
         <v>2</v>
       </c>
       <c r="D197">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E197">
         <v>5</v>
@@ -6495,7 +6495,7 @@
         <v>2</v>
       </c>
       <c r="D198">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E198">
         <v>3</v>
@@ -6526,7 +6526,7 @@
         <v>2</v>
       </c>
       <c r="D199">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E199">
         <v>4</v>
@@ -6557,7 +6557,7 @@
         <v>2</v>
       </c>
       <c r="D200">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -6588,7 +6588,7 @@
         <v>2</v>
       </c>
       <c r="D201">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E201">
         <v>2</v>
@@ -6619,7 +6619,7 @@
         <v>2</v>
       </c>
       <c r="D202">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E202">
         <v>2</v>
@@ -6650,7 +6650,7 @@
         <v>2</v>
       </c>
       <c r="D203">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E203">
         <v>2</v>
@@ -6681,7 +6681,7 @@
         <v>2</v>
       </c>
       <c r="D204">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E204">
         <v>5</v>

</xml_diff>